<commit_message>
Do radio and dropdown action from excel data
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -11,18 +11,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>test123</t>
+    <t>No</t>
   </si>
   <si>
-    <t>second test</t>
-  </si>
-  <si>
-    <t>3rd test</t>
-  </si>
-  <si>
-    <t>test 5</t>
+    <t>Mango</t>
   </si>
 </sst>
 </file>
@@ -56,11 +50,10 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
@@ -287,23 +280,14 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
+    <row r="2" ht="15.75" customHeight="1"/>
+    <row r="3" ht="15.75" customHeight="1"/>
     <row r="4" ht="15.75" customHeight="1"/>
-    <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
+    <row r="5" ht="15.75" customHeight="1"/>
     <row r="6" ht="15.75" customHeight="1"/>
     <row r="7" ht="15.75" customHeight="1"/>
     <row r="8" ht="15.75" customHeight="1"/>

</xml_diff>